<commit_message>
add teams names to html web page
add teams names to html web page
</commit_message>
<xml_diff>
--- a/statistics/statictics.xlsx
+++ b/statistics/statictics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eilon\Documents\eilon-learnings\final-project\ChameleonVISION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eilon\Documents\eilon-learnings\final-project\ChameleonVISION\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F87AFC7-247A-4D61-B790-09DE926A4EF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D2066B-BE0C-4676-9E7D-A0E8311287CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,16 +60,16 @@
     <t>herzelia</t>
   </si>
   <si>
-    <t>Itay</t>
-  </si>
-  <si>
-    <t>Eilon</t>
-  </si>
-  <si>
     <t>Herzelia</t>
   </si>
   <si>
     <t>shinny</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Brazil</t>
   </si>
 </sst>
 </file>
@@ -415,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -467,19 +467,19 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E2" s="3">
         <v>44241</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1">
         <v>65</v>

</xml_diff>

<commit_message>
add display of bar chart
</commit_message>
<xml_diff>
--- a/statistics/statictics.xlsx
+++ b/statistics/statictics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eilon\Documents\eilon-learnings\final-project\ChameleonVISION\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D2066B-BE0C-4676-9E7D-A0E8311287CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825516A5-8BF1-4895-82A8-6A6EB427C0AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,21 +416,20 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="7" max="7" width="33.08984375" customWidth="1"/>
-    <col min="8" max="8" width="33.1796875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="7" max="8" width="33.140625" customWidth="1"/>
     <col min="9" max="9" width="35" customWidth="1"/>
-    <col min="10" max="10" width="34.1796875" customWidth="1"/>
+    <col min="10" max="10" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -462,7 +461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -494,7 +493,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -506,7 +505,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -518,7 +517,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>

<commit_message>
show wide data from db into second html table
</commit_message>
<xml_diff>
--- a/statistics/statictics.xlsx
+++ b/statistics/statictics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eilon\Documents\eilon-learnings\final-project\ChameleonVISION\statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ChameleonVISION\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825516A5-8BF1-4895-82A8-6A6EB427C0AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A7E3AC-3D72-4A83-A07E-E1A079D18618}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,21 +415,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="7" max="8" width="33.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="7" max="8" width="33.1796875" customWidth="1"/>
     <col min="9" max="9" width="35" customWidth="1"/>
-    <col min="10" max="10" width="36.140625" customWidth="1"/>
+    <col min="10" max="10" width="36.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -461,7 +461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -481,19 +481,19 @@
         <v>12</v>
       </c>
       <c r="G2" s="1">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="H2" s="1">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="I2" s="1">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="J2" s="1">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -505,7 +505,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -517,7 +517,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>

</xml_diff>

<commit_message>
add line graph for second page
</commit_message>
<xml_diff>
--- a/statistics/statictics.xlsx
+++ b/statistics/statictics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ChameleonVISION\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A7E3AC-3D72-4A83-A07E-E1A079D18618}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AAA94E-D9C1-4216-89A4-969A513C8B25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added system accuracy  to page 1
</commit_message>
<xml_diff>
--- a/statistics/statictics.xlsx
+++ b/statistics/statictics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ChameleonVISION\statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eilon\Documents\eilon-learnings\final-project\ChameleonVISION\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AAA94E-D9C1-4216-89A4-969A513C8B25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3BAA76-42A9-480A-A482-D49EDAAEA3EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>GameName</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Brazil</t>
+  </si>
+  <si>
+    <t>SystemAccuracy</t>
   </si>
 </sst>
 </file>
@@ -128,11 +131,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -427,9 +431,10 @@
     <col min="7" max="8" width="33.1796875" customWidth="1"/>
     <col min="9" max="9" width="35" customWidth="1"/>
     <col min="10" max="10" width="36.1796875" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -460,8 +465,11 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -492,8 +500,11 @@
       <c r="J2" s="1">
         <v>37</v>
       </c>
+      <c r="K2" s="4">
+        <v>87</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -504,8 +515,9 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -516,8 +528,9 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -528,6 +541,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added dynamic percentage of system accuracy
</commit_message>
<xml_diff>
--- a/statistics/statictics.xlsx
+++ b/statistics/statictics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eilon\Documents\eilon-learnings\final-project\ChameleonVISION\statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ChameleonVISION\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3BAA76-42A9-480A-A482-D49EDAAEA3EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4106A3-28A3-4A0F-B9A8-F29BFD70EC05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>GameName</t>
   </si>
@@ -69,10 +69,13 @@
     <t>Israel</t>
   </si>
   <si>
-    <t>Brazil</t>
-  </si>
-  <si>
     <t>SystemAccuracy</t>
+  </si>
+  <si>
+    <t>2021-25-04</t>
+  </si>
+  <si>
+    <t>Turkey</t>
   </si>
 </sst>
 </file>
@@ -131,12 +134,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -431,7 +433,7 @@
     <col min="7" max="8" width="33.1796875" customWidth="1"/>
     <col min="9" max="9" width="35" customWidth="1"/>
     <col min="10" max="10" width="36.1796875" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -466,7 +468,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -477,13 +479,13 @@
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3">
-        <v>44241</v>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>12</v>
@@ -500,8 +502,8 @@
       <c r="J2" s="1">
         <v>37</v>
       </c>
-      <c r="K2" s="4">
-        <v>87</v>
+      <c r="K2" s="1">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
add homepage for statistics and upload game
</commit_message>
<xml_diff>
--- a/statistics/statictics.xlsx
+++ b/statistics/statictics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ChameleonVISION\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4106A3-28A3-4A0F-B9A8-F29BFD70EC05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A90D8F8-0AA8-4AFE-A6F8-ED5E52964F71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -422,7 +422,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -503,7 +503,7 @@
         <v>37</v>
       </c>
       <c r="K2" s="1">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>